<commit_message>
Added HUD overlay displaying current slotted spells
</commit_message>
<xml_diff>
--- a/Implementation Docs/Spell Effects.xlsx
+++ b/Implementation Docs/Spell Effects.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="106">
   <si>
     <t>Speed</t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>15 seconds, 2</t>
+  </si>
+  <si>
+    <t>Spell Icon</t>
+  </si>
+  <si>
+    <t>Overlay</t>
   </si>
 </sst>
 </file>
@@ -404,7 +410,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="27">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -518,48 +536,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L16" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A1:L16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:N16" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A1:N16"/>
   <sortState ref="A2:L16">
     <sortCondition ref="A1:A16"/>
   </sortState>
-  <tableColumns count="12">
+  <tableColumns count="14">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Effect"/>
-    <tableColumn id="3" name="ID" dataDxfId="20"/>
-    <tableColumn id="4" name="Level I" dataDxfId="19"/>
-    <tableColumn id="5" name="Level II" dataDxfId="18"/>
-    <tableColumn id="6" name="Level III" dataDxfId="17"/>
-    <tableColumn id="7" name="Coded" dataDxfId="16"/>
-    <tableColumn id="8" name="Sorcery" dataDxfId="15"/>
-    <tableColumn id="9" name="Sorcery Storage" dataDxfId="14"/>
-    <tableColumn id="11" name="Spellcasting" dataDxfId="13"/>
-    <tableColumn id="12" name="Sync Packet" dataDxfId="12"/>
-    <tableColumn id="13" name="Sorcery GUI" dataDxfId="11"/>
+    <tableColumn id="3" name="ID" dataDxfId="24"/>
+    <tableColumn id="4" name="Level I" dataDxfId="23"/>
+    <tableColumn id="5" name="Level II" dataDxfId="22"/>
+    <tableColumn id="6" name="Level III" dataDxfId="21"/>
+    <tableColumn id="7" name="Coded" dataDxfId="20"/>
+    <tableColumn id="8" name="Sorcery" dataDxfId="19"/>
+    <tableColumn id="9" name="Sorcery Storage" dataDxfId="18"/>
+    <tableColumn id="11" name="Spellcasting" dataDxfId="17"/>
+    <tableColumn id="12" name="Sync Packet" dataDxfId="16"/>
+    <tableColumn id="13" name="Sorcery GUI" dataDxfId="15"/>
+    <tableColumn id="10" name="Spell Icon" dataDxfId="3"/>
+    <tableColumn id="14" name="Overlay" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L9" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A1:L9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:N9" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:N9"/>
   <sortState ref="A2:M28">
     <sortCondition ref="A1:A28"/>
   </sortState>
-  <tableColumns count="12">
+  <tableColumns count="14">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Effect"/>
-    <tableColumn id="3" name="ID" dataDxfId="9"/>
-    <tableColumn id="4" name="Level I" dataDxfId="8"/>
-    <tableColumn id="5" name="Level II" dataDxfId="7"/>
-    <tableColumn id="6" name="Level III" dataDxfId="6"/>
-    <tableColumn id="7" name="Coded" dataDxfId="5"/>
-    <tableColumn id="8" name="Sorcery" dataDxfId="4"/>
-    <tableColumn id="9" name="Sorcery Storage" dataDxfId="3"/>
-    <tableColumn id="11" name="Spellcasting" dataDxfId="2"/>
-    <tableColumn id="12" name="Sync Packet" dataDxfId="1"/>
-    <tableColumn id="13" name="Sorcery GUI" dataDxfId="0"/>
+    <tableColumn id="3" name="ID" dataDxfId="13"/>
+    <tableColumn id="4" name="Level I" dataDxfId="12"/>
+    <tableColumn id="5" name="Level II" dataDxfId="11"/>
+    <tableColumn id="6" name="Level III" dataDxfId="10"/>
+    <tableColumn id="7" name="Coded" dataDxfId="9"/>
+    <tableColumn id="8" name="Sorcery" dataDxfId="8"/>
+    <tableColumn id="9" name="Sorcery Storage" dataDxfId="7"/>
+    <tableColumn id="11" name="Spellcasting" dataDxfId="6"/>
+    <tableColumn id="12" name="Sync Packet" dataDxfId="5"/>
+    <tableColumn id="13" name="Sorcery GUI" dataDxfId="4"/>
+    <tableColumn id="10" name="Spell Icon" dataDxfId="1"/>
+    <tableColumn id="14" name="Overlay" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -828,7 +850,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -838,20 +860,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -888,8 +912,14 @@
       <c r="L1" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -926,8 +956,14 @@
       <c r="L2" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -964,8 +1000,14 @@
       <c r="L3" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1002,8 +1044,14 @@
       <c r="L4" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1040,8 +1088,14 @@
       <c r="L5" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1078,8 +1132,14 @@
       <c r="L6" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1116,8 +1176,14 @@
       <c r="L7" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1154,8 +1220,14 @@
       <c r="L8" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1192,8 +1264,14 @@
       <c r="L9" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1230,8 +1308,14 @@
       <c r="L10" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1268,8 +1352,14 @@
       <c r="L11" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1306,8 +1396,14 @@
       <c r="L12" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1344,8 +1440,14 @@
       <c r="L13" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1382,8 +1484,14 @@
       <c r="L14" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1420,8 +1528,14 @@
       <c r="L15" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1456,6 +1570,12 @@
         <v>28</v>
       </c>
       <c r="L16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1470,7 +1590,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1480,19 +1600,21 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="18.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="16" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1529,8 +1651,14 @@
       <c r="L1" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1567,8 +1695,14 @@
       <c r="L2" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1605,8 +1739,14 @@
       <c r="L3" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1643,8 +1783,14 @@
       <c r="L4" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1681,8 +1827,14 @@
       <c r="L5" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1719,8 +1871,14 @@
       <c r="L6" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1757,8 +1915,14 @@
       <c r="L7" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1795,8 +1959,14 @@
       <c r="L8" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1831,6 +2001,12 @@
         <v>28</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>